<commit_message>
added new repair strategy "CREATE_IF_MISSING"
</commit_message>
<xml_diff>
--- a/resources/script/mapping/sampleMapping/Sample Mappings 06.xlsx
+++ b/resources/script/mapping/sampleMapping/Sample Mappings 06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sagportal-my.sharepoint.com/personal/ck_softwareag_com/Documents/intern/Products/Cumulocity/solutions/generic-mqtt-mapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{5005D566-A020-684D-A16B-C68C68329918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A3E5AC1-B714-8041-A773-B43BCF5A428F}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{5005D566-A020-684D-A16B-C68C68329918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC86109A-1BCF-AE4F-9174-2BB7B9D73C3C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{B5E387B2-3E90-884E-B546-D827ECD68714}"/>
   </bookViews>
@@ -695,14 +695,6 @@
   </si>
   <si>
     <t>{
-     "temperature": 120.5,
-     "unit": "Celsius",
-     "time": "2023-07-12T16:21:53.389+02:00",
-     "externalId": "berlin_01"
-}</t>
-  </si>
-  <si>
-    <t>{
     "source": {
        "id": "909090"
     },
@@ -713,10 +705,6 @@
 }</t>
   </si>
   <si>
-    <t>A measasurement should be created for the device berlin_01.
-The fragment "c8y_Fragment_to_remove" is not included in the created measurement, as the repair strategy is "REMOVE_IF_NULL".</t>
-  </si>
-  <si>
     <t>Mapping Type</t>
   </si>
   <si>
@@ -761,6 +749,20 @@
   </si>
   <si>
     <t>Hex Code: 5a75207370c3a47420303821</t>
+  </si>
+  <si>
+    <t>{
+     "temperature": 120.5,
+     "unit": "Celsius",
+     "time": "2023-07-12T16:21:53.389+02:00",
+     "externalId": "berlin_01",
+     "unexpected": 17.5
+}</t>
+  </si>
+  <si>
+    <t>A measasurement should be created for the device berlin_01.
+The fragment "c8y_Fragment_to_remove" is not included in the created measurement, as the repair strategy is "REMOVE_IF_NULL".
+In addition the reapar strategy "CREATE_IF_MISSING" is used. Thjsi is required to map the node "unexpected" to the target fragment "c8y_Unexpected". This is created, due to the used reapir strategy.</t>
   </si>
 </sst>
 </file>
@@ -1229,8 +1231,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="142" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="142" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1249,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1267,12 +1269,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>48</v>
@@ -1290,12 +1292,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>51</v>
@@ -1318,7 +1320,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>61</v>
@@ -1341,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>17</v>
@@ -1364,7 +1366,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>21</v>
@@ -1387,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>46</v>
@@ -1410,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>62</v>
@@ -1433,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>68</v>
@@ -1456,7 +1458,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>52</v>
@@ -1479,19 +1481,19 @@
         <v>13</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G11" s="24" t="s">
         <v>58</v>
@@ -1502,7 +1504,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>55</v>
@@ -1525,7 +1527,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>24</v>
@@ -1548,7 +1550,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>44</v>
@@ -1571,7 +1573,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>43</v>
@@ -1594,7 +1596,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>34</v>
@@ -1617,7 +1619,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>71</v>
@@ -1640,7 +1642,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>75</v>
@@ -1663,7 +1665,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>70</v>
@@ -1681,27 +1683,27 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="168" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="252" x14ac:dyDescent="0.2">
       <c r="A20" s="22">
         <v>25</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="23" t="s">
-        <v>78</v>
-      </c>
       <c r="G20" s="20" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>